<commit_message>
qdrant data complience content added
</commit_message>
<xml_diff>
--- a/poc/Project_plan_local_gtp.xlsx
+++ b/poc/Project_plan_local_gtp.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\app\rag-policies\poc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84107F2-5DC1-4217-85A3-CC531B5E8CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C306605D-BD24-4A59-A507-8F70D9E92339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F1E390A2-6E39-4801-814A-AB9A00E28921}"/>
+    <workbookView xWindow="28965" yWindow="1860" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{F1E390A2-6E39-4801-814A-AB9A00E28921}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Plan" sheetId="1" r:id="rId1"/>
-    <sheet name="Хөдөлмөрийн дотоод журам" sheetId="2" r:id="rId2"/>
-    <sheet name="МТ-ы үйл ажиллагаа" sheetId="3" r:id="rId3"/>
+    <sheet name="Комплайнс хариуцсан нэгжийн үаж" sheetId="4" r:id="rId2"/>
+    <sheet name="Хөдөлмөрийн дотоод журам" sheetId="2" r:id="rId3"/>
+    <sheet name="МТ-ы үйл ажиллагаа" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <t>Гол архитектур (өдөр тутмын үзэл)</t>
   </si>
@@ -429,6 +430,90 @@
   </si>
   <si>
     <t>End Data</t>
+  </si>
+  <si>
+    <t>. Ерөнхий ойлголт</t>
+  </si>
+  <si>
+    <t>Комплаенс хариуцсан нэгжийн үндсэн зорилго юу вэ?</t>
+  </si>
+  <si>
+    <t>“Комплаенс” гэж яг юуг хэлдэг вэ?</t>
+  </si>
+  <si>
+    <t>Комплаенсын соёл гэж юу вэ, ажилтан бүр яагаад мөрдөх ёстой вэ?</t>
+  </si>
+  <si>
+    <t>Комплаенсын эрсдэл гэж ямар эрсдэлийг хэлдэг вэ?</t>
+  </si>
+  <si>
+    <t>2. Чиг үүрэг, хамрах хүрээ</t>
+  </si>
+  <si>
+    <t>Комплаенс хариуцсан нэгж ямар чиг үүрэгтэй вэ?</t>
+  </si>
+  <si>
+    <t>Комплаенсийн бодлого, журамтай нийцүүлэн ажиллахад ажилтнуудын оролцоо ямар байх вэ?</t>
+  </si>
+  <si>
+    <t>Мөнгө угаах болон терроризмыг санхүүжүүлэхтэй тэмцэх (МУТСТ) үйл ажиллагааг ямар нэгж хариуцдаг вэ?</t>
+  </si>
+  <si>
+    <t>НҮБ болон олон улсын хориг арга хэмжээг хэрхэн хэрэгжүүлдэг вэ?</t>
+  </si>
+  <si>
+    <t>3. Ажилтны үүрэг, оролцоо</t>
+  </si>
+  <si>
+    <t>Ажилтнууд өдөр тутмын үйл ажиллагаандаа ямар комплаенсын зарчмуудыг мөрдөх ёстой вэ?</t>
+  </si>
+  <si>
+    <t>Ашиг сонирхлын зөрчил илэрвэл ажилтан яах ёстой вэ?</t>
+  </si>
+  <si>
+    <t>Харилцагчийн мэдээллийн нууцлалыг хамгаалахад ямар шаардлага тавигддаг вэ?</t>
+  </si>
+  <si>
+    <t>Зөрчил, дутагдал илрүүлсэн бол хаана мэдээлэх ёстой вэ?</t>
+  </si>
+  <si>
+    <t>4. Эрсдэлийн удирдлага</t>
+  </si>
+  <si>
+    <t>Комплаенсын эрсдэлийг хэрхэн үнэлдэг вэ?</t>
+  </si>
+  <si>
+    <t>Шинэ бүтээгдэхүүн, үйлчилгээ нэвтрүүлэх үед комплаенсын ямар үнэлгээ, санал шаардлагатай вэ?</t>
+  </si>
+  <si>
+    <t>Сэжигтэй гүйлгээг илрүүлсэн тохиолдолд яах ёстой вэ?</t>
+  </si>
+  <si>
+    <t>Өндөр эрсдэлтэй харилцагч болон улс оронтой холбоотой гүйлгээг хэрхэн хянадаг вэ?</t>
+  </si>
+  <si>
+    <t>5. Тайлагнал, хяналт</t>
+  </si>
+  <si>
+    <t>Комплаенсийн нэгж хэнд, хэдэн удаа тайлагнадаг вэ?</t>
+  </si>
+  <si>
+    <t>МУТСТ-тай холбоотой тайланг хаана, ямар хугацаанд хүргүүлдэг вэ?</t>
+  </si>
+  <si>
+    <t>Дотоод аудит комплаенсын үйл ажиллагаанд ямар хяналт тавьдаг вэ?</t>
+  </si>
+  <si>
+    <t>6. Хариуцлага</t>
+  </si>
+  <si>
+    <t>Комплаенсын журмыг зөрчвөл ямар хариуцлага хүлээх вэ?</t>
+  </si>
+  <si>
+    <t>Худал тайлан, буруу мэдээлэл хүргүүлбэл ямар үр дагавартай вэ?</t>
+  </si>
+  <si>
+    <t>Хөдөлмөрийн сахилгын шийтгэл хуулийн бусад хариуцлагаас чөлөөлөх үү?</t>
   </si>
 </sst>
 </file>
@@ -492,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -525,6 +610,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,7 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D9D9D1-96D5-4829-BD75-7FB8F1690B31}">
   <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1484,11 +1578,235 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC2FF8B-29BF-47E0-ADCC-4A2C1610F91A}">
+  <dimension ref="B1:B55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="B1" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="14"/>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="14"/>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="14"/>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="14"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="14"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="14"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="14"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="14"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="B31" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="14"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="14"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="14"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="14"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="B41" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="14"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="14"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="14"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="B49" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="14"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="14"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="14"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EB12EB-8938-425D-8506-45E68A7C7B29}">
   <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1610,7 +1928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFC21A4-1B28-445A-87F1-05947E81457C}">
   <dimension ref="A1:A61"/>
   <sheetViews>

</xml_diff>